<commit_message>
updated concepts in specs to NOV-16 + fixes
- The CSV source files have been downloaded and updated to match the
  most recent meeting on NOV-16. RDF+HTML has been generated. The new
  concepts (rights, rules, etc.) have NOT been included.
- fixes #72 broken link in DPV HTML
- fixes #58 incorrect labels
- fixes #70 typos in terms
- resolves #59 adding owl:import to DPV-OWL specs
- resolves #42 adding Machester syntax serializations for DPV-OWL
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/entities.xlsx
+++ b/documentation-generator/vocab_csv/entities.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="304">
   <si>
     <t>Term</t>
   </si>
@@ -217,6 +217,15 @@
   </si>
   <si>
     <t>https://www.w3.org/2022/03/02-dpvcg-minutes.html</t>
+  </si>
+  <si>
+    <t>isRepresentativeFor</t>
+  </si>
+  <si>
+    <t>is representative for</t>
+  </si>
+  <si>
+    <t>Indicates the entity is a representative for specified entity</t>
   </si>
   <si>
     <t>Authority</t>
@@ -5342,6 +5351,54 @@
       <c r="AA7" s="14"/>
       <c r="AB7" s="14"/>
     </row>
+    <row r="8">
+      <c r="A8" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15">
+        <v>44874.0</v>
+      </c>
+      <c r="L8" s="14"/>
+      <c r="M8" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="14"/>
+      <c r="AB8" s="14"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="O7">
     <cfRule type="expression" dxfId="2" priority="1">
@@ -5453,16 +5510,16 @@
     </row>
     <row r="2">
       <c r="A2" s="43" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D2" s="45" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E2" s="46" t="s">
         <v>26</v>
@@ -5480,7 +5537,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="44" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="O2" s="49" t="s">
         <v>37</v>
@@ -5501,16 +5558,16 @@
     </row>
     <row r="3">
       <c r="A3" s="43" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D3" s="44" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E3" s="51" t="s">
         <v>26</v>
@@ -5528,7 +5585,7 @@
         <v>19</v>
       </c>
       <c r="N3" s="44" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="O3" s="49" t="s">
         <v>37</v>
@@ -5549,16 +5606,16 @@
     </row>
     <row r="4">
       <c r="A4" s="44" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C4" s="51" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D4" s="44" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>26</v>
@@ -5568,7 +5625,7 @@
       <c r="H4" s="23"/>
       <c r="I4" s="52"/>
       <c r="J4" s="53" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K4" s="48">
         <v>44594.0</v>
@@ -5599,16 +5656,16 @@
     </row>
     <row r="5">
       <c r="A5" s="50" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C5" s="51" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>26</v>
@@ -5618,7 +5675,7 @@
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
       <c r="J5" s="53" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="K5" s="48">
         <v>44594.0</v>
@@ -5649,16 +5706,16 @@
     </row>
     <row r="6">
       <c r="A6" s="44" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C6" s="51" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D6" s="44" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>26</v>
@@ -5668,7 +5725,7 @@
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
       <c r="J6" s="54" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K6" s="48">
         <v>44594.0</v>
@@ -8582,19 +8639,19 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D2" s="33" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F2" s="39"/>
       <c r="G2" s="34"/>
@@ -8609,10 +8666,10 @@
         <v>19</v>
       </c>
       <c r="N2" s="33" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="O2" s="38" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="P2" s="39"/>
       <c r="Q2" s="39"/>
@@ -8630,16 +8687,16 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>17</v>
@@ -8657,10 +8714,10 @@
         <v>19</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="O3" s="38" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
@@ -8784,13 +8841,13 @@
     </row>
     <row r="2">
       <c r="A2" s="55" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C2" s="57" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D2" s="55" t="s">
         <v>34</v>
@@ -8802,10 +8859,10 @@
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
       <c r="I2" s="21" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="J2" s="58" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="K2" s="25">
         <v>43560.0</v>
@@ -8817,7 +8874,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="55" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="O2" s="27" t="s">
         <v>27</v>
@@ -8838,16 +8895,16 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>26</v>
@@ -8857,7 +8914,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="59" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="K3" s="15">
         <v>43620.0</v>
@@ -8870,7 +8927,7 @@
         <v>20</v>
       </c>
       <c r="O3" s="41" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
@@ -8888,16 +8945,16 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>26</v>
@@ -8906,7 +8963,7 @@
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="60" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="J4" s="14"/>
       <c r="K4" s="15">
@@ -8920,7 +8977,7 @@
         <v>20</v>
       </c>
       <c r="O4" s="41" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
@@ -8938,13 +8995,13 @@
     </row>
     <row r="5">
       <c r="A5" s="55" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B5" s="56" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C5" s="57" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D5" s="55" t="s">
         <v>34</v>
@@ -8954,16 +9011,16 @@
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="21" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="I5" s="62" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J5" s="63" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="K5" s="25">
         <v>43560.0</v>
@@ -8975,7 +9032,7 @@
         <v>19</v>
       </c>
       <c r="N5" s="55" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="O5" s="27" t="s">
         <v>27</v>
@@ -8996,16 +9053,16 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>26</v>
@@ -9015,7 +9072,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="59" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="K6" s="15">
         <v>43620.0</v>
@@ -9028,7 +9085,7 @@
         <v>20</v>
       </c>
       <c r="O6" s="41" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
@@ -9046,13 +9103,13 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>34</v>
@@ -9064,10 +9121,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="13" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="J7" s="64" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="K7" s="15">
         <v>44447.0</v>
@@ -9077,10 +9134,10 @@
         <v>19</v>
       </c>
       <c r="N7" s="33" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="O7" s="41" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
@@ -9098,16 +9155,16 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>26</v>
@@ -9116,10 +9173,10 @@
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
       <c r="I8" s="65" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="J8" s="64" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="K8" s="15">
         <v>44447.0</v>
@@ -9129,10 +9186,10 @@
         <v>19</v>
       </c>
       <c r="N8" s="33" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="O8" s="41" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
@@ -9150,16 +9207,16 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>26</v>
@@ -9168,7 +9225,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="13" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="J9" s="14"/>
       <c r="K9" s="15">
@@ -9179,7 +9236,7 @@
         <v>19</v>
       </c>
       <c r="N9" s="33" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="O9" s="41" t="s">
         <v>21</v>
@@ -9200,13 +9257,13 @@
     </row>
     <row r="10">
       <c r="A10" s="66" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B10" s="66" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C10" s="67" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D10" s="68" t="s">
         <v>60</v>
@@ -9219,7 +9276,7 @@
       <c r="H10" s="70"/>
       <c r="I10" s="70"/>
       <c r="J10" s="71" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="K10" s="72">
         <v>44139.0</v>
@@ -9228,10 +9285,10 @@
         <v>44538.0</v>
       </c>
       <c r="M10" s="73" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="N10" s="67" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="O10" s="74" t="s">
         <v>37</v>
@@ -9353,13 +9410,13 @@
     </row>
     <row r="2">
       <c r="A2" s="76" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B2" s="76" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C2" s="77" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D2" s="76" t="s">
         <v>17</v>
@@ -9385,7 +9442,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="76" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="O2" s="79" t="s">
         <v>27</v>
@@ -9406,22 +9463,22 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F3" s="80" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
@@ -9435,7 +9492,7 @@
         <v>19</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="O3" s="82" t="s">
         <v>31</v>
@@ -9456,22 +9513,22 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F4" s="80" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G4" s="23"/>
       <c r="H4" s="23"/>
@@ -9485,7 +9542,7 @@
         <v>19</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="O4" s="82" t="s">
         <v>31</v>
@@ -9506,19 +9563,19 @@
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>61</v>
@@ -9527,7 +9584,7 @@
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="13" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="K5" s="15">
         <v>43559.0</v>
@@ -9539,7 +9596,7 @@
         <v>19</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="O5" s="41" t="s">
         <v>27</v>
@@ -9560,22 +9617,22 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F6" s="80" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
@@ -9589,7 +9646,7 @@
         <v>19</v>
       </c>
       <c r="N6" s="21" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="O6" s="82" t="s">
         <v>31</v>
@@ -9610,22 +9667,22 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="F7" s="80" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
@@ -9639,7 +9696,7 @@
         <v>19</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="O7" s="82" t="s">
         <v>31</v>
@@ -9660,19 +9717,19 @@
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="F8" s="21" t="s">
         <v>61</v>
@@ -9689,7 +9746,7 @@
         <v>19</v>
       </c>
       <c r="N8" s="21" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="O8" s="82" t="s">
         <v>31</v>
@@ -9710,22 +9767,22 @@
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F9" s="80" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
@@ -9739,7 +9796,7 @@
         <v>19</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="O9" s="82" t="s">
         <v>31</v>
@@ -9760,22 +9817,22 @@
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="F10" s="80" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
@@ -9789,7 +9846,7 @@
         <v>19</v>
       </c>
       <c r="N10" s="21" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="O10" s="82" t="s">
         <v>65</v>
@@ -9903,11 +9960,11 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="13" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D2" s="33"/>
       <c r="E2" s="33"/>
@@ -9919,7 +9976,7 @@
       <c r="K2" s="36"/>
       <c r="L2" s="36"/>
       <c r="M2" s="33" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="N2" s="33"/>
       <c r="O2" s="33"/>
@@ -9939,13 +9996,13 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B3" s="76" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>34</v>
@@ -9987,16 +10044,16 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B4" s="76" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D4" s="80" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>26</v>
@@ -10006,7 +10063,7 @@
       <c r="H4" s="23"/>
       <c r="I4" s="23"/>
       <c r="J4" s="21" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="K4" s="25">
         <v>44594.0</v>
@@ -10015,7 +10072,7 @@
         <v>44109.0</v>
       </c>
       <c r="M4" s="61" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="N4" s="21" t="s">
         <v>20</v>
@@ -10039,16 +10096,16 @@
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C5" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" s="80" t="s">
         <v>193</v>
-      </c>
-      <c r="D5" s="80" t="s">
-        <v>190</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>26</v>
@@ -10065,7 +10122,7 @@
         <v>44109.0</v>
       </c>
       <c r="M5" s="61" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="N5" s="21" t="s">
         <v>20</v>
@@ -10089,16 +10146,16 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B6" s="76" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D6" s="80" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>26</v>
@@ -10108,7 +10165,7 @@
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
       <c r="J6" s="21" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="K6" s="25">
         <v>44594.0</v>
@@ -10117,7 +10174,7 @@
         <v>44109.0</v>
       </c>
       <c r="M6" s="61" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="N6" s="21" t="s">
         <v>20</v>
@@ -10141,16 +10198,16 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B7" s="76" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D7" s="80" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>26</v>
@@ -10167,7 +10224,7 @@
         <v>44109.0</v>
       </c>
       <c r="M7" s="61" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="N7" s="21" t="s">
         <v>20</v>
@@ -10191,16 +10248,16 @@
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B8" s="76" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D8" s="80" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>26</v>
@@ -10210,7 +10267,7 @@
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
       <c r="J8" s="21" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="K8" s="25">
         <v>44594.0</v>
@@ -10219,7 +10276,7 @@
         <v>44109.0</v>
       </c>
       <c r="M8" s="61" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="N8" s="21" t="s">
         <v>20</v>
@@ -10243,16 +10300,16 @@
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B9" s="76" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D9" s="80" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>26</v>
@@ -10262,7 +10319,7 @@
       <c r="H9" s="23"/>
       <c r="I9" s="23"/>
       <c r="J9" s="21" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="K9" s="25">
         <v>44594.0</v>
@@ -10271,7 +10328,7 @@
         <v>44109.0</v>
       </c>
       <c r="M9" s="61" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="N9" s="21" t="s">
         <v>20</v>
@@ -10295,16 +10352,16 @@
     </row>
     <row r="10">
       <c r="A10" s="44" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D10" s="45" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E10" s="22" t="s">
         <v>26</v>
@@ -10314,7 +10371,7 @@
       <c r="H10" s="23"/>
       <c r="I10" s="23"/>
       <c r="J10" s="53" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="K10" s="48">
         <v>44643.0</v>
@@ -10323,13 +10380,13 @@
         <v>44109.0</v>
       </c>
       <c r="M10" s="51" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="N10" s="44" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="O10" s="84" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="P10" s="28"/>
       <c r="Q10" s="28"/>
@@ -10347,13 +10404,13 @@
     </row>
     <row r="11">
       <c r="A11" s="44" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C11" s="45" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>25</v>
@@ -10374,10 +10431,10 @@
         <v>19</v>
       </c>
       <c r="N11" s="44" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="O11" s="84" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="P11" s="28"/>
       <c r="Q11" s="28"/>
@@ -10483,13 +10540,13 @@
     </row>
     <row r="2">
       <c r="A2" s="76" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B2" s="76" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C2" s="76" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D2" s="76" t="s">
         <v>17</v>
@@ -10515,7 +10572,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="76" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="O2" s="79" t="s">
         <v>27</v>
@@ -10536,13 +10593,13 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>17</v>
@@ -10556,7 +10613,7 @@
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
       <c r="M3" s="13" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="N3" s="13" t="s">
         <v>20</v>
@@ -10578,13 +10635,13 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>25</v>
@@ -10607,10 +10664,10 @@
         <v>19</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="O4" s="41" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
@@ -10719,16 +10776,16 @@
     </row>
     <row r="2">
       <c r="A2" s="56" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C2" s="85" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D2" s="86" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E2" s="87" t="s">
         <v>26</v>
@@ -10737,10 +10794,10 @@
       <c r="G2" s="28"/>
       <c r="H2" s="23"/>
       <c r="I2" s="56" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="J2" s="88" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="K2" s="78">
         <v>43560.0</v>
@@ -10752,7 +10809,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="89" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="O2" s="90" t="s">
         <v>27</v>
@@ -10773,16 +10830,16 @@
     </row>
     <row r="3">
       <c r="A3" s="55" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C3" s="55" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D3" s="61" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E3" s="87" t="s">
         <v>26</v>
@@ -10791,7 +10848,7 @@
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
       <c r="I3" s="91" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="J3" s="23"/>
       <c r="K3" s="25">
@@ -10801,13 +10858,13 @@
         <v>44734.0</v>
       </c>
       <c r="M3" s="61" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="N3" s="55" t="s">
         <v>20</v>
       </c>
       <c r="O3" s="91" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="P3" s="28"/>
       <c r="Q3" s="28"/>
@@ -10825,16 +10882,16 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>234</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>231</v>
       </c>
       <c r="E4" s="87" t="s">
         <v>26</v>
@@ -10852,10 +10909,10 @@
         <v>19</v>
       </c>
       <c r="N4" s="33" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="O4" s="41" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
@@ -10873,16 +10930,16 @@
     </row>
     <row r="5">
       <c r="A5" s="55" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B5" s="56" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C5" s="55" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D5" s="55" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E5" s="87" t="s">
         <v>26</v>
@@ -10891,7 +10948,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="93" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="J5" s="55"/>
       <c r="K5" s="25">
@@ -10902,7 +10959,7 @@
         <v>19</v>
       </c>
       <c r="N5" s="55" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="O5" s="91" t="s">
         <v>37</v>
@@ -10923,16 +10980,16 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E6" s="87" t="s">
         <v>26</v>
@@ -10950,10 +11007,10 @@
         <v>19</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="O6" s="41" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
@@ -10971,16 +11028,16 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E7" s="87" t="s">
         <v>26</v>
@@ -10998,10 +11055,10 @@
         <v>19</v>
       </c>
       <c r="N7" s="13" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="O7" s="41" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
@@ -11019,16 +11076,16 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E8" s="87" t="s">
         <v>26</v>
@@ -11046,10 +11103,10 @@
         <v>19</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="O8" s="41" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
@@ -11067,16 +11124,16 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E9" s="87" t="s">
         <v>26</v>
@@ -11094,10 +11151,10 @@
         <v>19</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="O9" s="41" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P9" s="14"/>
       <c r="Q9" s="14"/>
@@ -11115,16 +11172,16 @@
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E10" s="87" t="s">
         <v>26</v>
@@ -11142,10 +11199,10 @@
         <v>19</v>
       </c>
       <c r="N10" s="13" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="O10" s="41" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P10" s="14"/>
       <c r="Q10" s="14"/>
@@ -11163,16 +11220,16 @@
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E11" s="87" t="s">
         <v>26</v>
@@ -11190,10 +11247,10 @@
         <v>19</v>
       </c>
       <c r="N11" s="13" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="O11" s="41" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P11" s="14"/>
       <c r="Q11" s="14"/>
@@ -11211,16 +11268,16 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E12" s="87" t="s">
         <v>26</v>
@@ -11238,10 +11295,10 @@
         <v>19</v>
       </c>
       <c r="N12" s="13" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="O12" s="41" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P12" s="14"/>
       <c r="Q12" s="14"/>
@@ -11259,16 +11316,16 @@
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="D13" s="94" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E13" s="87" t="s">
         <v>26</v>
@@ -11277,7 +11334,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="13" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="J13" s="14"/>
       <c r="K13" s="15">
@@ -11288,10 +11345,10 @@
         <v>19</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="O13" s="41" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
@@ -11309,16 +11366,16 @@
     </row>
     <row r="14">
       <c r="A14" s="13" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E14" s="87" t="s">
         <v>26</v>
@@ -11336,10 +11393,10 @@
         <v>19</v>
       </c>
       <c r="N14" s="13" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="O14" s="41" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P14" s="14"/>
       <c r="Q14" s="14"/>
@@ -11357,16 +11414,16 @@
     </row>
     <row r="15">
       <c r="A15" s="13" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E15" s="87" t="s">
         <v>26</v>
@@ -11384,10 +11441,10 @@
         <v>19</v>
       </c>
       <c r="N15" s="13" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="O15" s="41" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
@@ -11405,16 +11462,16 @@
     </row>
     <row r="16">
       <c r="A16" s="13" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="E16" s="87" t="s">
         <v>26</v>
@@ -11432,10 +11489,10 @@
         <v>19</v>
       </c>
       <c r="N16" s="13" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="O16" s="41" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P16" s="14"/>
       <c r="Q16" s="14"/>
@@ -11453,16 +11510,16 @@
     </row>
     <row r="17">
       <c r="A17" s="13" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E17" s="87" t="s">
         <v>26</v>
@@ -11480,10 +11537,10 @@
         <v>19</v>
       </c>
       <c r="N17" s="13" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="O17" s="41" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P17" s="14"/>
       <c r="Q17" s="14"/>
@@ -11501,16 +11558,16 @@
     </row>
     <row r="18">
       <c r="A18" s="13" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E18" s="87" t="s">
         <v>26</v>
@@ -11528,10 +11585,10 @@
         <v>19</v>
       </c>
       <c r="N18" s="13" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="O18" s="41" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P18" s="14"/>
       <c r="Q18" s="14"/>
@@ -11549,16 +11606,16 @@
     </row>
     <row r="19">
       <c r="A19" s="13" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E19" s="87" t="s">
         <v>26</v>
@@ -11576,10 +11633,10 @@
         <v>19</v>
       </c>
       <c r="N19" s="13" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="O19" s="41" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P19" s="14"/>
       <c r="Q19" s="14"/>
@@ -11597,16 +11654,16 @@
     </row>
     <row r="20">
       <c r="A20" s="13" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E20" s="87" t="s">
         <v>26</v>
@@ -11615,7 +11672,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="13" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="J20" s="14"/>
       <c r="K20" s="15">
@@ -11626,10 +11683,10 @@
         <v>19</v>
       </c>
       <c r="N20" s="13" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="O20" s="41" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P20" s="14"/>
       <c r="Q20" s="14"/>
@@ -11647,16 +11704,16 @@
     </row>
     <row r="21">
       <c r="A21" s="13" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E21" s="87" t="s">
         <v>26</v>
@@ -11674,10 +11731,10 @@
         <v>19</v>
       </c>
       <c r="N21" s="13" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="O21" s="41" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P21" s="14"/>
       <c r="Q21" s="14"/>
@@ -11695,16 +11752,16 @@
     </row>
     <row r="22">
       <c r="A22" s="13" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E22" s="87" t="s">
         <v>26</v>
@@ -11722,10 +11779,10 @@
         <v>19</v>
       </c>
       <c r="N22" s="13" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="O22" s="41" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P22" s="14"/>
       <c r="Q22" s="14"/>
@@ -11743,16 +11800,16 @@
     </row>
     <row r="23">
       <c r="A23" s="13" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="E23" s="87" t="s">
         <v>26</v>
@@ -11770,10 +11827,10 @@
         <v>19</v>
       </c>
       <c r="N23" s="13" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="O23" s="41" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
@@ -11791,16 +11848,16 @@
     </row>
     <row r="24">
       <c r="A24" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="D24" s="13" t="s">
         <v>288</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>285</v>
       </c>
       <c r="E24" s="87" t="s">
         <v>26</v>
@@ -11818,10 +11875,10 @@
         <v>19</v>
       </c>
       <c r="N24" s="13" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="O24" s="41" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="P24" s="14"/>
       <c r="Q24" s="14"/>
@@ -11839,16 +11896,16 @@
     </row>
     <row r="25">
       <c r="A25" s="13" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="E25" s="87" t="s">
         <v>26</v>
@@ -11866,10 +11923,10 @@
         <v>19</v>
       </c>
       <c r="N25" s="13" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="O25" s="41" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="P25" s="14"/>
       <c r="Q25" s="14"/>
@@ -11887,16 +11944,16 @@
     </row>
     <row r="26">
       <c r="A26" s="13" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E26" s="87" t="s">
         <v>26</v>
@@ -11914,10 +11971,10 @@
         <v>19</v>
       </c>
       <c r="N26" s="13" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="O26" s="41" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="P26" s="14"/>
       <c r="Q26" s="14"/>
@@ -11935,16 +11992,16 @@
     </row>
     <row r="27">
       <c r="A27" s="13" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E27" s="87" t="s">
         <v>26</v>
@@ -11962,10 +12019,10 @@
         <v>19</v>
       </c>
       <c r="N27" s="13" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="O27" s="41" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="P27" s="14"/>
       <c r="Q27" s="14"/>

</xml_diff>